<commit_message>
Update timeline project plan.xlsx
</commit_message>
<xml_diff>
--- a/2. Schedulers/1. Project Plan/timeline project plan.xlsx
+++ b/2. Schedulers/1. Project Plan/timeline project plan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75311FE-EC59-4396-85EF-0F36A6400F89}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F6BA8A-1622-48F2-88DF-302ABB73351C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1741,7 +1741,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomLeft" activeCell="Y33" sqref="Y33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3344,7 +3344,7 @@
       </c>
       <c r="E26" s="68"/>
       <c r="F26" s="73">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="G26" s="74">
         <v>44993</v>
@@ -3405,7 +3405,7 @@
       <c r="D27" s="90"/>
       <c r="E27" s="68"/>
       <c r="F27" s="73">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G27" s="74">
         <f>H26+1</f>

</xml_diff>